<commit_message>
Add sleep turn feature
</commit_message>
<xml_diff>
--- a/BetterSleep/translations.xlsx
+++ b/BetterSleep/translations.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$D$20</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -334,6 +337,57 @@
   <si>
     <t xml:space="preserve">启用或禁用在冥想时随时睡觉的能力。</t>
   </si>
+  <si>
+    <t xml:space="preserve">topic03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleep Delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">睡眠ディレイ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">睡眠延迟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable Sleep Delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">睡眠ディレイを有効化</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用睡眠延迟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tooltip06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable turns delay before falling asleep.
+Set the number of turns it takes before the player character fully falls asleep.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">プレイヤーキャラクターが完全に眠るまでのターンディレイを有効または無効にします。
+眠りに入るまでに必要なターン数を設定します。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">启用或禁用入睡前的回合延迟。
+设置玩家角色完全入睡所需的回合数。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slider02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turn(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ターン数</t>
+  </si>
+  <si>
+    <t xml:space="preserve">回合数</t>
+  </si>
 </sst>
 </file>
 
@@ -342,7 +396,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -372,12 +426,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Microsoft YaHei"/>
+      <name val="Noto Sans SC"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -444,11 +493,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -461,7 +510,20 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -575,10 +637,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -618,7 +684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -632,7 +698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -646,7 +712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -674,7 +740,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -688,7 +754,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -702,7 +768,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="4" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -716,7 +782,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -730,7 +796,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -744,7 +810,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
@@ -758,7 +824,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -772,7 +838,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -786,7 +852,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
@@ -814,7 +880,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
@@ -828,7 +894,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
@@ -842,7 +908,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -852,7 +918,7 @@
       <c r="C19" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="3" t="s">
         <v>75</v>
       </c>
     </row>
@@ -863,14 +929,71 @@
       <c r="B20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>79</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D20"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -878,5 +1001,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>